<commit_message>
added some tests to test treasure cards
test that treasure cards don't add anything they shouldn't. Test that
treasure cards add money. Test that treasure cards don't use actions.
</commit_message>
<xml_diff>
--- a/Time Planning.xlsx
+++ b/Time Planning.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="2520" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>code coverage</t>
   </si>
@@ -83,6 +83,111 @@
   </si>
   <si>
     <t>random then modify cards</t>
+  </si>
+  <si>
+    <t>Text Cards to implement:</t>
+  </si>
+  <si>
+    <t>Adventurer</t>
+  </si>
+  <si>
+    <t>Bureaucrat</t>
+  </si>
+  <si>
+    <t>Cellar</t>
+  </si>
+  <si>
+    <t>Chancellor</t>
+  </si>
+  <si>
+    <t>Chapel</t>
+  </si>
+  <si>
+    <t>Council Room</t>
+  </si>
+  <si>
+    <t>Feast</t>
+  </si>
+  <si>
+    <t>Gardens</t>
+  </si>
+  <si>
+    <t>Library</t>
+  </si>
+  <si>
+    <t>Militia</t>
+  </si>
+  <si>
+    <t>Mine</t>
+  </si>
+  <si>
+    <t>Moat</t>
+  </si>
+  <si>
+    <t>Money Lender</t>
+  </si>
+  <si>
+    <t>Remodel</t>
+  </si>
+  <si>
+    <t>Spy</t>
+  </si>
+  <si>
+    <t>Thief</t>
+  </si>
+  <si>
+    <t>Throne Room</t>
+  </si>
+  <si>
+    <t>Witch</t>
+  </si>
+  <si>
+    <t>Workshop</t>
+  </si>
+  <si>
+    <t>Finished Cards:</t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Estate</t>
+  </si>
+  <si>
+    <t>Duchy</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>Festival</t>
+  </si>
+  <si>
+    <t>Laboratory</t>
+  </si>
+  <si>
+    <t>Market</t>
+  </si>
+  <si>
+    <t>Smithy</t>
+  </si>
+  <si>
+    <t>Village</t>
+  </si>
+  <si>
+    <t>Woodcutter</t>
+  </si>
+  <si>
+    <t>percent finished</t>
+  </si>
+  <si>
+    <t>number finished</t>
   </si>
 </sst>
 </file>
@@ -433,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -445,10 +550,10 @@
     <col min="2" max="2" width="22.5546875" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="26.5546875" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
@@ -462,7 +567,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>5</v>
       </c>
@@ -476,7 +581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>6</v>
       </c>
@@ -490,7 +595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>7</v>
       </c>
@@ -507,7 +612,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>8</v>
       </c>
@@ -521,7 +626,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>9</v>
       </c>
@@ -535,7 +640,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>10</v>
       </c>
@@ -547,6 +652,168 @@
       </c>
       <c r="E7" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10">
+        <f>(F9 / 31) * 100</f>
+        <v>19.35483870967742</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" t="s">
+        <v>51</v>
+      </c>
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C29" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moved some tests into Visual Studio Framework
</commit_message>
<xml_diff>
--- a/Time Planning.xlsx
+++ b/Time Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3636" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="4812" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,7 +541,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,7 +603,7 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
@@ -620,7 +620,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E5" t="s">
         <v>18</v>
@@ -634,7 +634,7 @@
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
made some tests to test bureaucrat. (all fail)
</commit_message>
<xml_diff>
--- a/Time Planning.xlsx
+++ b/Time Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4812" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="5988" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,9 +705,6 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
       <c r="D14" t="s">
         <v>52</v>
       </c>
@@ -740,14 +737,20 @@
       <c r="C18" t="s">
         <v>33</v>
       </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>34</v>
       </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>35</v>
       </c>
     </row>
@@ -776,43 +779,38 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>41</v>
-      </c>
-    </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated that some cards are now working
</commit_message>
<xml_diff>
--- a/Time Planning.xlsx
+++ b/Time Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4812" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="5988" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -540,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -705,9 +705,6 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C14" t="s">
-        <v>29</v>
-      </c>
       <c r="D14" t="s">
         <v>52</v>
       </c>
@@ -740,14 +737,20 @@
       <c r="C18" t="s">
         <v>33</v>
       </c>
+      <c r="D18" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>34</v>
       </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>35</v>
       </c>
     </row>
@@ -776,43 +779,38 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C26" t="s">
-        <v>41</v>
-      </c>
-    </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C27" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C29" t="s">
+      <c r="D29" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C33" t="s">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D33" t="s">
         <v>46</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated time planning completed cards
</commit_message>
<xml_diff>
--- a/Time Planning.xlsx
+++ b/Time Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5988" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="7188" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -541,7 +541,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,9 +658,6 @@
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" s="1" t="s">
         <v>43</v>
       </c>
@@ -672,8 +669,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>25</v>
+      <c r="D10" t="s">
+        <v>24</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>56</v>
@@ -687,6 +684,9 @@
       <c r="C11" t="s">
         <v>26</v>
       </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
@@ -726,9 +726,6 @@
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
       <c r="D17" t="s">
         <v>55</v>
       </c>
@@ -757,6 +754,9 @@
     <row r="21" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>36</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated time planning sheet
</commit_message>
<xml_diff>
--- a/Time Planning.xlsx
+++ b/Time Planning.xlsx
@@ -541,7 +541,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -672,9 +672,6 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
       <c r="E10" s="1" t="s">
         <v>56</v>
       </c>
@@ -718,9 +715,6 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C16" t="s">
-        <v>31</v>
-      </c>
       <c r="D16" t="s">
         <v>54</v>
       </c>
@@ -758,10 +752,16 @@
       <c r="C21" t="s">
         <v>36</v>
       </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Updated problem statement and time planning sheet
</commit_message>
<xml_diff>
--- a/Time Planning.xlsx
+++ b/Time Planning.xlsx
@@ -541,7 +541,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,9 +658,6 @@
       <c r="B9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" s="1" t="s">
         <v>43</v>
       </c>
@@ -672,6 +669,9 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>56</v>
       </c>
@@ -684,6 +684,9 @@
       <c r="C11" t="s">
         <v>26</v>
       </c>
+      <c r="D11" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
@@ -694,9 +697,6 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
       <c r="D13" t="s">
         <v>51</v>
       </c>
@@ -720,9 +720,6 @@
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
       <c r="D17" t="s">
         <v>55</v>
       </c>
@@ -736,9 +733,6 @@
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C19" t="s">
-        <v>34</v>
-      </c>
       <c r="D19" t="s">
         <v>29</v>
       </c>
@@ -768,15 +762,21 @@
       <c r="C23" t="s">
         <v>38</v>
       </c>
+      <c r="D23" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C24" t="s">
         <v>39</v>
       </c>
+      <c r="D24" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C25" t="s">
-        <v>40</v>
+      <c r="D25" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added tests for feast
</commit_message>
<xml_diff>
--- a/Time Planning.xlsx
+++ b/Time Planning.xlsx
@@ -541,7 +541,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -751,9 +751,6 @@
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C22" t="s">
-        <v>37</v>
-      </c>
       <c r="D22" t="s">
         <v>25</v>
       </c>
@@ -779,9 +776,14 @@
         <v>28</v>
       </c>
     </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>42</v>
+      </c>
+    </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C27" t="s">
-        <v>42</v>
+      <c r="D27" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update time planning (newly implemented cards)
</commit_message>
<xml_diff>
--- a/Time Planning.xlsx
+++ b/Time Planning.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="5988" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="7188" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -538,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,9 +716,6 @@
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
       <c r="D18" t="s">
         <v>41</v>
       </c>
@@ -734,9 +731,6 @@
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C21" t="s">
-        <v>36</v>
-      </c>
       <c r="D21" t="s">
         <v>31</v>
       </c>
@@ -747,9 +741,6 @@
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C23" t="s">
-        <v>38</v>
-      </c>
       <c r="D23" t="s">
         <v>34</v>
       </c>
@@ -820,6 +811,21 @@
     <row r="36" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D36" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D37" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D39" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>